<commit_message>
mod ini thershold, create new exccel file
</commit_message>
<xml_diff>
--- a/LogParser/LTE.xlsx
+++ b/LogParser/LTE.xlsx
@@ -885,14 +885,14 @@
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
     <cfRule type="cellIs" priority="1" operator="notBetween" dxfId="0" stopIfTrue="1">
-      <formula>100</formula>
-      <formula>-100</formula>
+      <formula>-15</formula>
+      <formula>-16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C10">
     <cfRule type="cellIs" priority="2" operator="notBetween" dxfId="0" stopIfTrue="1">
-      <formula>100</formula>
-      <formula>-100</formula>
+      <formula>-28</formula>
+      <formula>-29</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1317,19 +1317,19 @@
   </sheetData>
   <conditionalFormatting sqref="B2:B10">
     <cfRule type="cellIs" priority="1" operator="notBetween" dxfId="0" stopIfTrue="1">
-      <formula>100</formula>
+      <formula>21</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C10">
     <cfRule type="cellIs" priority="2" operator="notBetween" dxfId="0" stopIfTrue="1">
-      <formula>100</formula>
+      <formula>22.5</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="3" operator="notBetween" dxfId="0" stopIfTrue="1">
-      <formula>100</formula>
+      <formula>31.5</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
modify logic for reading logs
</commit_message>
<xml_diff>
--- a/LogParser/LTE.xlsx
+++ b/LogParser/LTE.xlsx
@@ -7,10 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="LTE_Power_Current" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="LTE_LAN" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Zigbee_Current" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Zigbee_dBm" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Zigbee_Power_Current" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Zigbee_LAN" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="LTE_Current" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="LTE_dBm" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -471,51 +471,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5891801300008_0727181606</t>
+          <t>5891801300001_0731161805</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v/>
+        <v>9.442</v>
       </c>
       <c r="C2" t="n">
-        <v/>
+        <v>9.688000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v/>
+        <v>8.916</v>
       </c>
       <c r="E2" t="n">
-        <v/>
+        <v>81</v>
       </c>
       <c r="F2" t="n">
-        <v/>
+        <v>82</v>
       </c>
       <c r="G2" t="n">
-        <v/>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5891801300005_0729063540</t>
+          <t>5891801300002_0731153739</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9.238</v>
+        <v>8.997999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>8.575000000000001</v>
+        <v>8.928000000000001</v>
       </c>
       <c r="D3" t="n">
-        <v>8.973000000000001</v>
+        <v>9.047000000000001</v>
       </c>
       <c r="E3" t="n">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F3" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G3" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
@@ -546,45 +546,45 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5891801300002_0731153739</t>
+          <t>5891801300004_0731153126</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8.997999999999999</v>
+        <v>9.665999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>8.928000000000001</v>
+        <v>8.817</v>
       </c>
       <c r="D5" t="n">
-        <v>9.047000000000001</v>
+        <v>9.260000000000002</v>
       </c>
       <c r="E5" t="n">
         <v>81</v>
       </c>
       <c r="F5" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G5" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5891801300009_0729031917</t>
+          <t>5891801300005_0729063540</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8.575999999999999</v>
+        <v>9.238</v>
       </c>
       <c r="C6" t="n">
-        <v>8.688000000000001</v>
+        <v>8.575000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>8.975000000000001</v>
+        <v>8.973000000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" t="n">
         <v>77</v>
@@ -596,101 +596,101 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>5891801300001_0731161805</t>
+          <t>5891801300006_0731155333</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9.442</v>
+        <v>8.622999999999999</v>
       </c>
       <c r="C7" t="n">
-        <v>9.688000000000001</v>
+        <v>8.923999999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>8.916</v>
+        <v>9.232000000000001</v>
       </c>
       <c r="E7" t="n">
+        <v>79</v>
+      </c>
+      <c r="F7" t="n">
+        <v>73</v>
+      </c>
+      <c r="G7" t="n">
         <v>81</v>
-      </c>
-      <c r="F7" t="n">
-        <v>82</v>
-      </c>
-      <c r="G7" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>5891801300004_0731153126</t>
+          <t>5891801300008_0727181606</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>9.665999999999999</v>
+        <v/>
       </c>
       <c r="C8" t="n">
-        <v>8.817</v>
+        <v/>
       </c>
       <c r="D8" t="n">
-        <v>9.260000000000002</v>
+        <v/>
       </c>
       <c r="E8" t="n">
-        <v>81</v>
+        <v/>
       </c>
       <c r="F8" t="n">
-        <v>81</v>
+        <v/>
       </c>
       <c r="G8" t="n">
-        <v>80</v>
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5891801300006_0731155333</t>
+          <t>5891801300008_0728214258</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8.622999999999999</v>
+        <v>9.257999999999999</v>
       </c>
       <c r="C9" t="n">
-        <v>8.923999999999999</v>
+        <v>9.426</v>
       </c>
       <c r="D9" t="n">
-        <v>9.232000000000001</v>
+        <v>8.617000000000001</v>
       </c>
       <c r="E9" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F9" t="n">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G9" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5891801300008_0728214258</t>
+          <t>5891801300009_0729031917</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9.257999999999999</v>
+        <v>8.575999999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>9.426</v>
+        <v>8.688000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>8.617000000000001</v>
+        <v>8.975000000000001</v>
       </c>
       <c r="E10" t="n">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F10" t="n">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G10" t="n">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -768,24 +768,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5891801300008_0727181606</t>
+          <t>5891801300001_0731161805</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v/>
+        <v>-15</v>
       </c>
       <c r="C2" t="n">
-        <v/>
+        <v>-28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5891801300005_0729063540</t>
+          <t>5891801300002_0731153739</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="C3" t="n">
         <v>-28</v>
@@ -807,37 +807,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5891801300002_0731153739</t>
+          <t>5891801300004_0731153126</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>-16</v>
       </c>
       <c r="C5" t="n">
-        <v>-28</v>
+        <v>-29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5891801300009_0729031917</t>
+          <t>5891801300005_0729063540</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-16</v>
+        <v>-15</v>
       </c>
       <c r="C6" t="n">
-        <v>-29</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>5891801300001_0731161805</t>
+          <t>5891801300006_0731155333</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="C7" t="n">
         <v>-28</v>
@@ -846,40 +846,40 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>5891801300004_0731153126</t>
+          <t>5891801300008_0727181606</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-16</v>
+        <v/>
       </c>
       <c r="C8" t="n">
-        <v>-29</v>
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5891801300006_0731155333</t>
+          <t>5891801300008_0728214258</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-16</v>
+        <v>-13</v>
       </c>
       <c r="C9" t="n">
-        <v>-28</v>
+        <v>-26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5891801300008_0728214258</t>
+          <t>5891801300009_0729031917</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-13</v>
+        <v>-16</v>
       </c>
       <c r="C10" t="n">
-        <v>-26</v>
+        <v>-29</v>
       </c>
     </row>
   </sheetData>
@@ -938,33 +938,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5891801300008_0727181606</t>
+          <t>5891801300001_0731161805</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>209</v>
+        <v>246</v>
       </c>
       <c r="C2" t="n">
-        <v>245</v>
+        <v>213</v>
       </c>
       <c r="D2" t="n">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5891801300005_0729063540</t>
+          <t>5891801300002_0731153739</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>213</v>
+        <v>252</v>
       </c>
       <c r="C3" t="n">
-        <v>251</v>
+        <v>211</v>
       </c>
       <c r="D3" t="n">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4">
@@ -974,10 +974,10 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>244</v>
+      </c>
+      <c r="C4" t="n">
         <v>204</v>
-      </c>
-      <c r="C4" t="n">
-        <v>244</v>
       </c>
       <c r="D4" t="n">
         <v>152</v>
@@ -986,97 +986,97 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5891801300002_0731153739</t>
+          <t>5891801300004_0731153126</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>211</v>
+        <v>241</v>
       </c>
       <c r="C5" t="n">
-        <v>252</v>
+        <v>205</v>
       </c>
       <c r="D5" t="n">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5891801300009_0729031917</t>
+          <t>5891801300005_0729063540</t>
         </is>
       </c>
       <c r="B6" t="n">
+        <v>251</v>
+      </c>
+      <c r="C6" t="n">
         <v>213</v>
       </c>
-      <c r="C6" t="n">
-        <v>243</v>
-      </c>
       <c r="D6" t="n">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>5891801300001_0731161805</t>
+          <t>5891801300006_0731155333</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>213</v>
+        <v>241</v>
       </c>
       <c r="C7" t="n">
-        <v>246</v>
+        <v>207</v>
       </c>
       <c r="D7" t="n">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>5891801300004_0731153126</t>
+          <t>5891801300008_0727181606</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>205</v>
+        <v>245</v>
       </c>
       <c r="C8" t="n">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="D8" t="n">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5891801300006_0731155333</t>
+          <t>5891801300008_0728214258</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>207</v>
+        <v>243</v>
       </c>
       <c r="C9" t="n">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="D9" t="n">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5891801300008_0728214258</t>
+          <t>5891801300009_0729031917</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>209</v>
+        <v>243</v>
       </c>
       <c r="C10" t="n">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D10" t="n">
-        <v>154</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1146,17 +1146,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5891801300008_0727181606</t>
+          <t>5891801300001_0731161805</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20.876</v>
+        <v>22.592</v>
       </c>
       <c r="C2" t="n">
-        <v>21.654</v>
+        <v>21.27</v>
       </c>
       <c r="D2" t="n">
-        <v>30.265</v>
+        <v>31.718</v>
       </c>
       <c r="E2" t="n">
         <v>-58</v>
@@ -1165,17 +1165,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5891801300005_0729063540</t>
+          <t>5891801300002_0731153739</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>20.841</v>
+        <v>23.126</v>
       </c>
       <c r="C3" t="n">
-        <v>23.045</v>
+        <v>21.759</v>
       </c>
       <c r="D3" t="n">
-        <v>31.558</v>
+        <v>31.393</v>
       </c>
       <c r="E3" t="n">
         <v>-58</v>
@@ -1188,32 +1188,32 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>23.071</v>
+      </c>
+      <c r="C4" t="n">
         <v>20.848</v>
-      </c>
-      <c r="C4" t="n">
-        <v>23.071</v>
       </c>
       <c r="D4" t="n">
         <v>31.622</v>
       </c>
       <c r="E4" t="n">
-        <v>-58</v>
+        <v>-588</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5891801300002_0731153739</t>
+          <t>5891801300004_0731153126</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21.759</v>
+        <v>22.453</v>
       </c>
       <c r="C5" t="n">
-        <v>23.126</v>
+        <v>21.119</v>
       </c>
       <c r="D5" t="n">
-        <v>31.393</v>
+        <v>31.638</v>
       </c>
       <c r="E5" t="n">
         <v>-58</v>
@@ -1222,17 +1222,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5891801300009_0729031917</t>
+          <t>5891801300005_0729063540</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.161</v>
+        <v>23.045</v>
       </c>
       <c r="C6" t="n">
-        <v>22.954</v>
+        <v>20.841</v>
       </c>
       <c r="D6" t="n">
-        <v>31.305</v>
+        <v>31.558</v>
       </c>
       <c r="E6" t="n">
         <v>-58</v>
@@ -1241,17 +1241,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>5891801300001_0731161805</t>
+          <t>5891801300006_0731155333</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>21.27</v>
+        <v>22.564</v>
       </c>
       <c r="C7" t="n">
-        <v>22.592</v>
+        <v>21.071</v>
       </c>
       <c r="D7" t="n">
-        <v>31.718</v>
+        <v>31.667</v>
       </c>
       <c r="E7" t="n">
         <v>-58</v>
@@ -1260,17 +1260,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>5891801300004_0731153126</t>
+          <t>5891801300008_0727181606</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>21.119</v>
+        <v>21.654</v>
       </c>
       <c r="C8" t="n">
-        <v>22.453</v>
+        <v>20.876</v>
       </c>
       <c r="D8" t="n">
-        <v>31.638</v>
+        <v>30.265</v>
       </c>
       <c r="E8" t="n">
         <v>-58</v>
@@ -1279,17 +1279,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5891801300006_0731155333</t>
+          <t>5891801300008_0728214258</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>21.071</v>
+        <v>23.047</v>
       </c>
       <c r="C9" t="n">
-        <v>22.564</v>
+        <v>20.811</v>
       </c>
       <c r="D9" t="n">
-        <v>31.667</v>
+        <v>31.579</v>
       </c>
       <c r="E9" t="n">
         <v>-58</v>
@@ -1298,17 +1298,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5891801300008_0728214258</t>
+          <t>5891801300009_0729031917</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>20.811</v>
+        <v>22.954</v>
       </c>
       <c r="C10" t="n">
-        <v>23.047</v>
+        <v>21.161</v>
       </c>
       <c r="D10" t="n">
-        <v>31.579</v>
+        <v>31.305</v>
       </c>
       <c r="E10" t="n">
         <v>-58</v>

</xml_diff>